<commit_message>
Implement Excel file management features: add upload and download routes in app.py, update admin panel for Excel management, and change branding from "Ettara Caffe" to "Ettarra Coffee House" in multiple templates.
</commit_message>
<xml_diff>
--- a/coffee_menu.xlsx
+++ b/coffee_menu.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Hackathon\internship\Day1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aniru\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B210625B-0A00-48D7-A058-0FF188990A98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86556C8C-A016-43EB-B5F0-38F8DC92067A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4284" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hot Coffee" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="76">
   <si>
     <t>Item Name</t>
   </si>
@@ -104,7 +104,16 @@
     <t>Flat white</t>
   </si>
   <si>
-    <t>Just The Way Our Australian Friends Like It "More Milk Less Drama"</t>
+    <t xml:space="preserve">Just The Way Our Australian Friends Like It </t>
+  </si>
+  <si>
+    <t>230</t>
+  </si>
+  <si>
+    <t>300</t>
+  </si>
+  <si>
+    <t>Cooling Special</t>
   </si>
   <si>
     <t>Cafe Mocha</t>
@@ -206,9 +215,6 @@
     <t>og_tart4.jpg</t>
   </si>
   <si>
-    <t>Cooling Special</t>
-  </si>
-  <si>
     <t>Matcha Frappe</t>
   </si>
   <si>
@@ -240,6 +246,12 @@
   </si>
   <si>
     <t>Cold Brew</t>
+  </si>
+  <si>
+    <t>Best selling</t>
+  </si>
+  <si>
+    <t>30% off</t>
   </si>
 </sst>
 </file>
@@ -605,7 +617,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -643,6 +655,9 @@
       <c r="E2" t="s">
         <v>8</v>
       </c>
+      <c r="F2" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -708,6 +723,9 @@
       <c r="E6" t="s">
         <v>8</v>
       </c>
+      <c r="F6" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -784,19 +802,25 @@
       <c r="B11" t="s">
         <v>26</v>
       </c>
-      <c r="C11">
-        <v>230</v>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" t="s">
+        <v>28</v>
       </c>
       <c r="E11" t="s">
         <v>8</v>
+      </c>
+      <c r="F11" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C12">
         <v>235</v>
@@ -810,10 +834,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C13">
         <v>275</v>
@@ -860,10 +884,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C2">
         <v>270</v>
@@ -877,10 +901,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C3">
         <v>300</v>
@@ -892,15 +916,15 @@
         <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C4">
         <v>350</v>
@@ -936,7 +960,7 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -947,10 +971,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C2">
         <v>185</v>
@@ -964,10 +988,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C3">
         <v>225</v>
@@ -981,10 +1005,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C4">
         <v>275</v>
@@ -998,10 +1022,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C5">
         <v>305</v>
@@ -1015,10 +1039,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C6">
         <v>305</v>
@@ -1032,10 +1056,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C7">
         <v>305</v>
@@ -1049,10 +1073,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C8">
         <v>305</v>
@@ -1066,10 +1090,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C9">
         <v>305</v>
@@ -1083,10 +1107,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C10">
         <v>305</v>
@@ -1100,10 +1124,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B11" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C11">
         <v>335</v>
@@ -1112,18 +1136,18 @@
         <v>375</v>
       </c>
       <c r="E11" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F11" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C12">
         <v>405</v>
@@ -1156,7 +1180,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -1167,10 +1191,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C2">
         <v>300</v>
@@ -1181,10 +1205,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C3">
         <v>300</v>
@@ -1214,7 +1238,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -1225,7 +1249,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C2">
         <v>250</v>
@@ -1236,7 +1260,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C3">
         <v>250</v>
@@ -1247,7 +1271,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C4">
         <v>250</v>
@@ -1258,7 +1282,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C5">
         <v>300</v>

</xml_diff>